<commit_message>
updated searchAny function (backend) updated User model (backend): email not null added Usability Test Report (work in progress)
</commit_message>
<xml_diff>
--- a/docs/Backend_Models.xlsx
+++ b/docs/Backend_Models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a5b6fa8fcd6b6a78/Dokumente/GitHub/ese2019-team8/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A85265C8-C4A2-49FD-90B3-0706BDFCBCE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{A85265C8-C4A2-49FD-90B3-0706BDFCBCE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0FB42F11-E5B7-4327-81FE-A56D937E9709}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{AF04898C-1559-41BF-989C-7A9BF9D0EB6F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Backend Models</t>
   </si>
@@ -584,6 +584,9 @@
       <c r="B10" t="s">
         <v>3</v>
       </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
updated search function (backend): not case-sensitive anymore added user manual (work in progress)
</commit_message>
<xml_diff>
--- a/docs/Backend_Models.xlsx
+++ b/docs/Backend_Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A85265C8-C4A2-49FD-90B3-0706BDFCBCE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0FB42F11-E5B7-4327-81FE-A56D937E9709}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{A85265C8-C4A2-49FD-90B3-0706BDFCBCE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{16F5D4F6-9BBA-4975-A7D6-D98DA7CF33DD}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{AF04898C-1559-41BF-989C-7A9BF9D0EB6F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>Backend Models</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>contactMail</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FADC19-1F1B-4D98-950F-454CD00969B0}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -691,44 +694,52 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated usability test report (graphs, layout etc.) slightly updated other documentation files
</commit_message>
<xml_diff>
--- a/docs/Backend_Models.xlsx
+++ b/docs/Backend_Models.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{A85265C8-C4A2-49FD-90B3-0706BDFCBCE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{16F5D4F6-9BBA-4975-A7D6-D98DA7CF33DD}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{A85265C8-C4A2-49FD-90B3-0706BDFCBCE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BE6B8952-B029-4673-857F-2453FA385FAC}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{AF04898C-1559-41BF-989C-7A9BF9D0EB6F}"/>
   </bookViews>
@@ -86,12 +86,6 @@
     <t>isAdmin</t>
   </si>
   <si>
-    <t>orange = not shown in "toSimplification"</t>
-  </si>
-  <si>
-    <t>yellow = no update via "fromSimplification"</t>
-  </si>
-  <si>
     <t>Service</t>
   </si>
   <si>
@@ -132,6 +126,12 @@
   </si>
   <si>
     <t>contactMail</t>
+  </si>
+  <si>
+    <t>olive green = no update via "fromSimplification"</t>
+  </si>
+  <si>
+    <t>aquamarine = not shown in "toSimplification"</t>
   </si>
 </sst>
 </file>
@@ -142,7 +142,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -150,7 +150,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -164,13 +164,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,8 +190,8 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -211,9 +211,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Metropolitan">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Metropolitan">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -221,48 +221,48 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="162F33"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EAF0E0"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="50B4C8"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="A8B97F"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9B9256"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="657689"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="7A855D"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="84AC9D"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="2370CD"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="877589"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Metropolitan">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -286,39 +286,22 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
         <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Cans" typeface="Euphemia"/>
@@ -335,29 +318,12 @@
         <a:font script="Laoo" typeface="DokChampa"/>
         <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Metropolitan">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -366,76 +332,73 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="70000"/>
+                <a:satMod val="100000"/>
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:tint val="75000"/>
+                <a:satMod val="101000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="82000"/>
+                <a:satMod val="104000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="2700000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
+                <a:tint val="97000"/>
+                <a:satMod val="100000"/>
                 <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="100000"/>
                 <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:shade val="80000"/>
+                <a:satMod val="100000"/>
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="2700000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -465,33 +428,12 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -499,7 +441,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Metropolitan" id="{4C5440D6-04D2-4954-96CF-F251137069B2}" vid="{79CFCA13-9412-4290-BB4B-85112F88857B}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,9 +456,9 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15.796875" customWidth="1"/>
-    <col min="2" max="2" width="7.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.06640625" customWidth="1"/>
+    <col min="3" max="3" width="15.3984375" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
@@ -525,25 +467,25 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -558,16 +500,16 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -635,36 +577,36 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
+      <c r="C19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
@@ -675,7 +617,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -683,18 +625,18 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -702,7 +644,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -713,7 +655,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -721,15 +663,15 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
@@ -737,7 +679,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>

</xml_diff>